<commit_message>
Adding to manual corrections and OG/OTH fuel types
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F13F406-77E9-4A3F-9248-2ABE4BD10FC8}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5C1FDF7-A633-4D2A-8722-CDE82C7F405F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>plant_id</t>
   </si>
@@ -97,12 +97,6 @@
     <t>lon</t>
   </si>
   <si>
-    <t>primary_fuel_type</t>
-  </si>
-  <si>
-    <t>primary_fuel_category</t>
-  </si>
-  <si>
     <t>GN35</t>
   </si>
   <si>
@@ -130,12 +124,6 @@
     <t>03</t>
   </si>
   <si>
-    <t>NG</t>
-  </si>
-  <si>
-    <t>GAS</t>
-  </si>
-  <si>
     <t>8.2</t>
   </si>
   <si>
@@ -158,6 +146,12 @@
   </si>
   <si>
     <t>GT</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -582,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -596,7 +590,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -610,7 +604,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -618,13 +612,13 @@
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -634,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="A24:E25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +761,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -849,7 +843,7 @@
         <v>50973</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -866,7 +860,7 @@
         <v>50973</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -883,7 +877,7 @@
         <v>50973</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -900,7 +894,7 @@
         <v>50973</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -917,7 +911,7 @@
         <v>50973</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -931,58 +925,86 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -993,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,50 +1127,6 @@
         <v>-81.042000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Addressing problem of duplicate generators without a general "slice(1)" since data may be lost this way.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{548FE47B-F7CC-4BFA-90AA-6EF8BFD94FFE}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3FBD15E-45B4-4DDB-9FD4-EE611C55C81B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>plant_id</t>
   </si>
@@ -97,12 +97,6 @@
     <t>lon</t>
   </si>
   <si>
-    <t>primary_fuel_type</t>
-  </si>
-  <si>
-    <t>primary_fuel_category</t>
-  </si>
-  <si>
     <t>GN35</t>
   </si>
   <si>
@@ -130,16 +124,37 @@
     <t>03</t>
   </si>
   <si>
-    <t>NG</t>
-  </si>
-  <si>
-    <t>GAS</t>
-  </si>
-  <si>
     <t>8.2</t>
   </si>
   <si>
     <t>8.1999999999999993</t>
+  </si>
+  <si>
+    <t>50489</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>keep_leading_zeroes</t>
   </si>
 </sst>
 </file>
@@ -528,16 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -566,7 +581,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -580,7 +595,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -594,7 +609,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,13 +617,21 @@
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>56032</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -618,10 +641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -833,7 +856,7 @@
         <v>50973</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -850,7 +873,7 @@
         <v>50973</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -867,7 +890,7 @@
         <v>50973</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -884,7 +907,7 @@
         <v>50973</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -901,7 +924,7 @@
         <v>50973</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -911,6 +934,90 @@
       </c>
       <c r="E19" s="3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -921,16 +1028,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="18.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1033,50 +1140,6 @@
         <v>-81.042000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating solution for duplicate generators with multiple prime movers.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3FBD15E-45B4-4DDB-9FD4-EE611C55C81B}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7162004-B790-4DBE-9004-77963F7DE4C6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
   <si>
     <t>plant_id</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>keep_leading_zeroes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -632,6 +638,34 @@
       </c>
       <c r="C6" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>55350</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>55350</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating solution for duplicate prime movers in generator file, updating names of QA files.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7162004-B790-4DBE-9004-77963F7DE4C6}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54B2948E-6E7C-4B8F-8517-52690545B408}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>plant_id</t>
   </si>
@@ -549,123 +549,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7512</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7512</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7512</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>56032</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>55350</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>55350</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating static tables to 2023.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5C1FDF7-A633-4D2A-8722-CDE82C7F405F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEB890F-F9C2-4943-829B-05A1A1754E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
   <si>
     <t>plant_id</t>
   </si>
@@ -544,14 +544,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7512</v>
       </c>
@@ -579,7 +579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7512</v>
       </c>
@@ -593,7 +593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7512</v>
       </c>
@@ -607,7 +607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>664</v>
       </c>
@@ -628,21 +628,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="3"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="3"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -659,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>55248</v>
       </c>
@@ -670,7 +670,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2847</v>
       </c>
@@ -681,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2707</v>
       </c>
@@ -695,7 +695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2707</v>
       </c>
@@ -709,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2707</v>
       </c>
@@ -723,7 +723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2707</v>
       </c>
@@ -737,45 +737,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>2132</v>
+        <v>7832</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>7832</v>
+        <v>7063</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>7063</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>50973</v>
+      </c>
+      <c r="B10" s="3">
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>50973</v>
       </c>
       <c r="B11" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -787,12 +796,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>50973</v>
       </c>
       <c r="B12" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -804,12 +813,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>50973</v>
       </c>
       <c r="B13" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -821,12 +830,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>50973</v>
       </c>
-      <c r="B14" s="3">
-        <v>44</v>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -838,12 +847,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>50973</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -855,12 +864,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>50973</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -872,12 +881,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>50973</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -889,12 +898,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>50973</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -906,29 +915,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>50973</v>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -937,12 +943,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -951,12 +957,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -965,45 +971,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1017,18 +1009,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="3"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>54975</v>
       </c>
@@ -1050,7 +1042,7 @@
         <v>32.380032</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>62262</v>
       </c>
@@ -1061,7 +1053,7 @@
         <v>42.899028999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>63003</v>
       </c>
@@ -1072,7 +1064,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>64850</v>
       </c>
@@ -1083,7 +1075,7 @@
         <v>36.168999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>54975</v>
       </c>
@@ -1094,7 +1086,7 @@
         <v>-106.753716</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>62262</v>
       </c>
@@ -1105,7 +1097,7 @@
         <v>-75.458455999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>63003</v>
       </c>
@@ -1116,7 +1108,7 @@
         <v>-89.996843999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>64850</v>
       </c>

</xml_diff>

<commit_message>
Updating static tables to 2023 data.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78856B84-9820-42DD-888C-D381CBF52D78}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20FD5158-9A71-437A-9ADA-857B90B12160}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
   <si>
     <t>plant_id</t>
   </si>
@@ -97,12 +97,6 @@
     <t>lon</t>
   </si>
   <si>
-    <t>primary_fuel_type</t>
-  </si>
-  <si>
-    <t>primary_fuel_category</t>
-  </si>
-  <si>
     <t>GN35</t>
   </si>
   <si>
@@ -130,16 +124,43 @@
     <t>03</t>
   </si>
   <si>
-    <t>NG</t>
-  </si>
-  <si>
-    <t>GAS</t>
-  </si>
-  <si>
     <t>8.2</t>
   </si>
   <si>
     <t>8.1999999999999993</t>
+  </si>
+  <si>
+    <t>50489</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>keep_leading_zeroes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -528,85 +549,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7512</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7512</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7512</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>56032</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>55350</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>55350</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -616,9 +685,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -725,7 +796,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
-        <v>2132</v>
+        <v>7832</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -733,27 +804,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <v>7832</v>
+        <v>7063</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
-        <v>7063</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>50973</v>
+      </c>
+      <c r="B10" s="3">
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -761,7 +841,7 @@
         <v>50973</v>
       </c>
       <c r="B11" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -778,7 +858,7 @@
         <v>50973</v>
       </c>
       <c r="B12" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -795,7 +875,7 @@
         <v>50973</v>
       </c>
       <c r="B13" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -811,8 +891,8 @@
       <c r="A14" s="3">
         <v>50973</v>
       </c>
-      <c r="B14" s="3">
-        <v>44</v>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -829,7 +909,7 @@
         <v>50973</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -846,7 +926,7 @@
         <v>50973</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -863,7 +943,7 @@
         <v>50973</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -880,7 +960,7 @@
         <v>50973</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -893,20 +973,87 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>50973</v>
+      <c r="A19" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -917,9 +1064,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1027,50 +1176,6 @@
         <v>-81.042000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>55970</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>10154</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating static tables for 2023.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEB890F-F9C2-4943-829B-05A1A1754E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20FD5158-9A71-437A-9ADA-857B90B12160}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
   <si>
     <t>plant_id</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>keep_leading_zeroes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -540,85 +549,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>7512</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>7512</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>7512</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>56032</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>55350</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>55350</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -631,18 +688,18 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="3"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7265625" style="3"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.08984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -659,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>55248</v>
       </c>
@@ -670,7 +727,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2847</v>
       </c>
@@ -681,7 +738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2707</v>
       </c>
@@ -695,7 +752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2707</v>
       </c>
@@ -709,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2707</v>
       </c>
@@ -723,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>2707</v>
       </c>
@@ -737,7 +794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7832</v>
       </c>
@@ -745,7 +802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7063</v>
       </c>
@@ -762,7 +819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>50973</v>
       </c>
@@ -779,7 +836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>50973</v>
       </c>
@@ -796,7 +853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>50973</v>
       </c>
@@ -813,7 +870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>50973</v>
       </c>
@@ -830,7 +887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>50973</v>
       </c>
@@ -847,7 +904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>50973</v>
       </c>
@@ -864,7 +921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>50973</v>
       </c>
@@ -881,7 +938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>50973</v>
       </c>
@@ -898,7 +955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>50973</v>
       </c>
@@ -915,7 +972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -929,7 +986,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -943,7 +1000,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -957,7 +1014,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -971,7 +1028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -985,7 +1042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1010,17 +1067,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="3"/>
-    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>54975</v>
       </c>
@@ -1042,7 +1099,7 @@
         <v>32.380032</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>62262</v>
       </c>
@@ -1053,7 +1110,7 @@
         <v>42.899028999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>63003</v>
       </c>
@@ -1064,7 +1121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>64850</v>
       </c>
@@ -1075,7 +1132,7 @@
         <v>36.168999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>54975</v>
       </c>
@@ -1086,7 +1143,7 @@
         <v>-106.753716</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>62262</v>
       </c>
@@ -1097,7 +1154,7 @@
         <v>-75.458455999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>63003</v>
       </c>
@@ -1108,7 +1165,7 @@
         <v>-89.996843999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>64850</v>
       </c>

</xml_diff>

<commit_message>
Updating manual_corrections via QA, updating unit file to include prime mover in IDs
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abtassoc-my.sharepoint.com/personal/teagan_goforth_abtassoc_com/Documents/Documents/eGRID/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{436F2B8E-15EB-4A2F-863A-726B680465AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20FD5158-9A71-437A-9ADA-857B90B12160}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBABF00A-6943-461A-8F31-D812482B6A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="generator_file" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>plant_id</t>
   </si>
@@ -95,21 +95,6 @@
   </si>
   <si>
     <t>lon</t>
-  </si>
-  <si>
-    <t>GN35</t>
-  </si>
-  <si>
-    <t>GN41</t>
-  </si>
-  <si>
-    <t>GN42</t>
-  </si>
-  <si>
-    <t>GN43</t>
-  </si>
-  <si>
-    <t>GN44</t>
   </si>
   <si>
     <t>OT</t>
@@ -555,15 +540,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7512</v>
       </c>
@@ -591,10 +576,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7512</v>
       </c>
@@ -605,10 +590,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7512</v>
       </c>
@@ -619,37 +604,37 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>664</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>56032</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>55350</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -658,15 +643,15 @@
         <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>55350</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -675,7 +660,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -685,21 +670,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="3"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="3"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -716,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>55248</v>
       </c>
@@ -727,7 +712,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2847</v>
       </c>
@@ -738,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2707</v>
       </c>
@@ -752,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2707</v>
       </c>
@@ -766,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2707</v>
       </c>
@@ -780,7 +765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2707</v>
       </c>
@@ -794,7 +779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7832</v>
       </c>
@@ -802,7 +787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7063</v>
       </c>
@@ -810,7 +795,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -819,241 +804,88 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B10" s="3">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B11" s="3">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B12" s="3">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B13" s="3">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>50973</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>50973</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>50973</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1070,14 +902,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="19.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="3"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>54975</v>
       </c>
@@ -1099,7 +931,7 @@
         <v>32.380032</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>62262</v>
       </c>
@@ -1110,7 +942,7 @@
         <v>42.899028999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>63003</v>
       </c>
@@ -1121,7 +953,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>64850</v>
       </c>
@@ -1132,7 +964,7 @@
         <v>36.168999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>54975</v>
       </c>
@@ -1143,7 +975,7 @@
         <v>-106.753716</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>62262</v>
       </c>
@@ -1154,7 +986,7 @@
         <v>-75.458455999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>63003</v>
       </c>
@@ -1165,7 +997,7 @@
         <v>-89.996843999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>64850</v>
       </c>

</xml_diff>

<commit_message>
Adding proposed plant to manual corrections and updating data cleaning steps with manual corrections, removing duplicate static table, adding maual corrections to unit file, updating generator file with EPA plants to delete and manual changes to fuel codes, fixing typo in generator file for calculating ozone generation for December plants.
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBABF00A-6943-461A-8F31-D812482B6A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EA647F-A614-402E-A363-56AE987A5288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="8580" yWindow="4140" windowWidth="14400" windowHeight="11460" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="generator_file" sheetId="2" r:id="rId1"/>
-    <sheet name="unit_file" sheetId="1" r:id="rId2"/>
-    <sheet name="plant_file" sheetId="3" r:id="rId3"/>
+    <sheet name="epa_clean" sheetId="5" r:id="rId1"/>
+    <sheet name="eia_clean" sheetId="6" r:id="rId2"/>
+    <sheet name="generator_file" sheetId="2" r:id="rId3"/>
+    <sheet name="unit_file" sheetId="1" r:id="rId4"/>
+    <sheet name="plant_file" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
   <si>
     <t>plant_id</t>
   </si>
@@ -146,6 +148,87 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>52152</t>
+  </si>
+  <si>
+    <t>6RB</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>heat_input</t>
+  </si>
+  <si>
+    <t>6413476.992</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2383097.20 </t>
+  </si>
+  <si>
+    <t>heat_input_oz</t>
+  </si>
+  <si>
+    <t>nox_mass</t>
+  </si>
+  <si>
+    <t>272.69</t>
+  </si>
+  <si>
+    <t>nox_oz_mass</t>
+  </si>
+  <si>
+    <t>97.016</t>
+  </si>
+  <si>
+    <t>so2_mass</t>
+  </si>
+  <si>
+    <t>1272.5545</t>
+  </si>
+  <si>
+    <t>co2_mass</t>
+  </si>
+  <si>
+    <t>608148.783</t>
+  </si>
+  <si>
+    <t>heat_input_source</t>
+  </si>
+  <si>
+    <t>EIA Prime Mover-level Data</t>
+  </si>
+  <si>
+    <t>heat_input_oz_source</t>
+  </si>
+  <si>
+    <t>nox_source</t>
+  </si>
+  <si>
+    <t>Estimated using emissions factor</t>
+  </si>
+  <si>
+    <t>nox_oz_source</t>
+  </si>
+  <si>
+    <t>so2_source</t>
+  </si>
+  <si>
+    <t>co2_source</t>
+  </si>
+  <si>
+    <t>operating_status</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>NPLPS</t>
+  </si>
+  <si>
+    <t>add</t>
   </si>
 </sst>
 </file>
@@ -533,11 +616,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D934C9D8-7DA6-4C13-BBA3-1B260AEBF0C8}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>880004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>57788</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD042B8F-EA7C-4084-B7F4-709825082C60}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60910</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791B152A-9A17-4C98-BF21-937C78FED9AB}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,25 +842,36 @@
         <v>34</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="E12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="3"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -886,6 +1076,210 @@
       </c>
       <c r="E15" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +1288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
   <dimension ref="A1:C9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding prime mover change to manual corrections for plant 6559, removing leading zeroes for matching on EIA-EPA crosswalk
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EA647F-A614-402E-A363-56AE987A5288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4544D677-AF72-457D-A488-55A35BEAFFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="4140" windowWidth="14400" windowHeight="11460" activeTab="1" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="11895" yWindow="870" windowWidth="14400" windowHeight="11460" firstSheet="1" activeTab="4" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="epa_clean" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
   <si>
     <t>plant_id</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>add</t>
+  </si>
+  <si>
+    <t>6559</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -672,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD042B8F-EA7C-4084-B7F4-709825082C60}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +722,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,10 +865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,6 +1288,23 @@
         <v>55</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,68 +1361,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>63003</v>
+        <v>54975</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>-106.753716</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>64850</v>
+        <v>62262</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>36.168999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>54975</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>-106.753716</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>62262</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
         <v>-75.458455999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>63003</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>-89.996843999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>64850</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>-81.042000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating manual corrections, abbreviating NOx controls
</commit_message>
<xml_diff>
--- a/data/static_tables/manual_corrections.xlsx
+++ b/data/static_tables/manual_corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\eGrid\production_model\users\gofortht\data\static_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4544D677-AF72-457D-A488-55A35BEAFFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD33EAC3-267A-4AFE-8CEA-24A070777F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11895" yWindow="870" windowWidth="14400" windowHeight="11460" firstSheet="1" activeTab="4" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{FA61C6A3-A5F8-4301-A228-D222830EB6CC}"/>
   </bookViews>
   <sheets>
     <sheet name="epa_clean" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
   <si>
     <t>plant_id</t>
   </si>
@@ -235,6 +235,42 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>6052</t>
+  </si>
+  <si>
+    <t>1745</t>
+  </si>
+  <si>
+    <t>67621</t>
+  </si>
+  <si>
+    <t>52193</t>
+  </si>
+  <si>
+    <t>21H</t>
+  </si>
+  <si>
+    <t>21H701</t>
+  </si>
+  <si>
+    <t>37H1</t>
+  </si>
+  <si>
+    <t>42H123</t>
+  </si>
+  <si>
+    <t>primary_fuel_type</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>MECCU1</t>
+  </si>
+  <si>
+    <t>MECCU2</t>
   </si>
 </sst>
 </file>
@@ -284,11 +320,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,16 +904,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1A8242-D17A-4DAB-8319-EC8C1026D049}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -984,48 +1022,36 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>7063</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
+      <c r="A9" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
+      <c r="A11" s="3">
+        <v>7063</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,7 +1059,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1047,7 +1073,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1064,10 +1090,10 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,44 +1104,38 @@
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,10 +1149,10 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,10 +1166,10 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,10 +1183,10 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,10 +1200,10 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,10 +1217,10 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,10 +1234,10 @@
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,10 +1251,10 @@
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,10 +1268,10 @@
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,7 +1285,7 @@
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>55</v>
@@ -1282,7 +1302,7 @@
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>55</v>
@@ -1290,19 +1310,155 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D30" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1313,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A26772A-0AAB-4516-99B5-5272EE829F50}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="F22:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1482,7 @@
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>54975</v>
       </c>
@@ -1348,7 +1504,7 @@
         <v>32.380032</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>62262</v>
       </c>
@@ -1359,7 +1515,7 @@
         <v>42.899028999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>54975</v>
       </c>
@@ -1370,7 +1526,7 @@
         <v>-106.753716</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>62262</v>
       </c>
@@ -1380,6 +1536,34 @@
       <c r="C5">
         <v>-75.458455999999998</v>
       </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>42.502749999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>-79.281723</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>